<commit_message>
added balanced accuracy based on reviewer feedback
</commit_message>
<xml_diff>
--- a/appendix/metrics_all_cap-sotu.xlsx
+++ b/appendix/metrics_all_cap-sotu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -893,7 +893,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>accuracy_balanced_mean</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -917,13 +917,13 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>0.446</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>accuracy_balanced_mean</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -932,28 +932,28 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>0.173</v>
       </c>
       <c r="D17" t="n">
-        <v>0.006</v>
+        <v>0.12</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01</v>
+        <v>0.173</v>
       </c>
       <c r="F17" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.185</v>
       </c>
       <c r="G17" t="n">
-        <v>0.017</v>
+        <v>0.216</v>
       </c>
       <c r="H17" t="n">
-        <v>0.013</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>accuracy_balanced_mean</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -962,28 +962,28 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.025</v>
+        <v>0.302</v>
       </c>
       <c r="D18" t="n">
-        <v>0.019</v>
+        <v>0.266</v>
       </c>
       <c r="E18" t="n">
-        <v>0.008</v>
+        <v>0.297</v>
       </c>
       <c r="F18" t="n">
-        <v>0.023</v>
+        <v>0.332</v>
       </c>
       <c r="G18" t="n">
-        <v>0.017</v>
+        <v>0.472</v>
       </c>
       <c r="H18" t="n">
-        <v>0.014</v>
+        <v>0.598</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>accuracy_balanced_mean</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -992,28 +992,28 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.008</v>
+        <v>0.346</v>
       </c>
       <c r="D19" t="n">
-        <v>0.008</v>
+        <v>0.348</v>
       </c>
       <c r="E19" t="n">
-        <v>0.005</v>
+        <v>0.348</v>
       </c>
       <c r="F19" t="n">
-        <v>0.011</v>
+        <v>0.401</v>
       </c>
       <c r="G19" t="n">
-        <v>0.016</v>
+        <v>0.524</v>
       </c>
       <c r="H19" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.644</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>accuracy_balanced_mean</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1022,28 +1022,28 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.002</v>
+        <v>0.375</v>
       </c>
       <c r="D20" t="n">
-        <v>0.001</v>
+        <v>0.406</v>
       </c>
       <c r="E20" t="n">
-        <v>0.012</v>
+        <v>0.395</v>
       </c>
       <c r="F20" t="n">
-        <v>0.003</v>
+        <v>0.489</v>
       </c>
       <c r="G20" t="n">
-        <v>0.015</v>
+        <v>0.626</v>
       </c>
       <c r="H20" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.668</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>accuracy_balanced_mean</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1052,28 +1052,28 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.004</v>
+        <v>0.378</v>
       </c>
       <c r="D21" t="n">
-        <v>0.002</v>
+        <v>0.427</v>
       </c>
       <c r="E21" t="n">
-        <v>0.007</v>
+        <v>0.429</v>
       </c>
       <c r="F21" t="n">
-        <v>0.007</v>
+        <v>0.54</v>
       </c>
       <c r="G21" t="n">
-        <v>0.011</v>
+        <v>0.681</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01</v>
+        <v>0.707</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>accuracy_balanced_mean</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1082,28 +1082,28 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.005</v>
+        <v>0.428</v>
       </c>
       <c r="D22" t="n">
-        <v>0.004</v>
+        <v>0.402</v>
       </c>
       <c r="E22" t="n">
-        <v>0.005</v>
+        <v>0.447</v>
       </c>
       <c r="F22" t="n">
-        <v>0.007</v>
+        <v>0.572</v>
       </c>
       <c r="G22" t="n">
-        <v>0.004</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="H22" t="n">
-        <v>0.017</v>
+        <v>0.722</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>f1_macro_std</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1133,7 +1133,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>f1_macro_std</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1142,28 +1142,28 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.014</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.012</v>
+        <v>0.006</v>
       </c>
       <c r="E24" t="n">
-        <v>0.016</v>
+        <v>0.01</v>
       </c>
       <c r="F24" t="n">
         <v>0.008999999999999999</v>
       </c>
       <c r="G24" t="n">
-        <v>0.02</v>
+        <v>0.017</v>
       </c>
       <c r="H24" t="n">
-        <v>0.016</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>f1_macro_std</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1172,28 +1172,28 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.012</v>
+        <v>0.025</v>
       </c>
       <c r="D25" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="H25" t="n">
         <v>0.014</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.012</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.015</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>f1_macro_std</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1202,28 +1202,28 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="D26" t="n">
-        <v>0.004</v>
+        <v>0.008</v>
       </c>
       <c r="E26" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="F26" t="n">
-        <v>0.003</v>
+        <v>0.011</v>
       </c>
       <c r="G26" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="H26" t="n">
-        <v>0.021</v>
+        <v>0.008999999999999999</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>f1_macro_std</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1232,28 +1232,28 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="D27" t="n">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
       <c r="E27" t="n">
-        <v>0.005</v>
+        <v>0.012</v>
       </c>
       <c r="F27" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="G27" t="n">
-        <v>0.004</v>
+        <v>0.015</v>
       </c>
       <c r="H27" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>f1_macro_std</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1265,16 +1265,16 @@
         <v>0.004</v>
       </c>
       <c r="D28" t="n">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="E28" t="n">
-        <v>0.005</v>
+        <v>0.007</v>
       </c>
       <c r="F28" t="n">
-        <v>0.001</v>
+        <v>0.007</v>
       </c>
       <c r="G28" t="n">
-        <v>0.008</v>
+        <v>0.011</v>
       </c>
       <c r="H28" t="n">
         <v>0.01</v>
@@ -1283,31 +1283,451 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
+          <t>f1_macro_std</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
           <t>f1_micro_std</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>10000</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="C36" t="n">
         <v>0.002</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D36" t="n">
         <v>0.002</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E36" t="n">
         <v>0.003</v>
       </c>
-      <c r="F29" t="n">
+      <c r="F36" t="n">
         <v>0.004</v>
       </c>
-      <c r="G29" t="n">
+      <c r="G36" t="n">
         <v>0.001</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H36" t="n">
         <v>0.007</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated appendix.py with many additional metrics and added many additional tables for each metric
</commit_message>
<xml_diff>
--- a/appendix/metrics_all_cap-sotu.xlsx
+++ b/appendix/metrics_all_cap-sotu.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -683,7 +683,7 @@
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_mean</t>
+          <t>accuracy/f1_micro_mean</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -713,7 +713,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_mean</t>
+          <t>accuracy/f1_micro_mean</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -743,7 +743,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_mean</t>
+          <t>accuracy/f1_micro_mean</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -773,7 +773,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_mean</t>
+          <t>accuracy/f1_micro_mean</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -803,7 +803,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_mean</t>
+          <t>accuracy/f1_micro_mean</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -833,7 +833,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_mean</t>
+          <t>accuracy/f1_micro_mean</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -863,7 +863,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_mean</t>
+          <t>accuracy/f1_micro_mean</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1103,7 +1103,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>recall_macro_mean</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1127,13 +1127,13 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0</v>
+        <v>0.446</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>recall_macro_mean</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1142,28 +1142,28 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>0.173</v>
       </c>
       <c r="D24" t="n">
-        <v>0.006</v>
+        <v>0.12</v>
       </c>
       <c r="E24" t="n">
-        <v>0.01</v>
+        <v>0.173</v>
       </c>
       <c r="F24" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.185</v>
       </c>
       <c r="G24" t="n">
-        <v>0.017</v>
+        <v>0.216</v>
       </c>
       <c r="H24" t="n">
-        <v>0.013</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>recall_macro_mean</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1172,28 +1172,28 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.025</v>
+        <v>0.302</v>
       </c>
       <c r="D25" t="n">
-        <v>0.019</v>
+        <v>0.266</v>
       </c>
       <c r="E25" t="n">
-        <v>0.008</v>
+        <v>0.297</v>
       </c>
       <c r="F25" t="n">
-        <v>0.023</v>
+        <v>0.332</v>
       </c>
       <c r="G25" t="n">
-        <v>0.017</v>
+        <v>0.472</v>
       </c>
       <c r="H25" t="n">
-        <v>0.014</v>
+        <v>0.598</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>recall_macro_mean</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1202,28 +1202,28 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.008</v>
+        <v>0.346</v>
       </c>
       <c r="D26" t="n">
-        <v>0.008</v>
+        <v>0.348</v>
       </c>
       <c r="E26" t="n">
-        <v>0.005</v>
+        <v>0.348</v>
       </c>
       <c r="F26" t="n">
-        <v>0.011</v>
+        <v>0.401</v>
       </c>
       <c r="G26" t="n">
-        <v>0.016</v>
+        <v>0.524</v>
       </c>
       <c r="H26" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.644</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>recall_macro_mean</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1232,28 +1232,28 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.002</v>
+        <v>0.375</v>
       </c>
       <c r="D27" t="n">
-        <v>0.001</v>
+        <v>0.406</v>
       </c>
       <c r="E27" t="n">
-        <v>0.012</v>
+        <v>0.395</v>
       </c>
       <c r="F27" t="n">
-        <v>0.003</v>
+        <v>0.489</v>
       </c>
       <c r="G27" t="n">
-        <v>0.015</v>
+        <v>0.626</v>
       </c>
       <c r="H27" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.668</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>recall_macro_mean</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1262,28 +1262,28 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.004</v>
+        <v>0.378</v>
       </c>
       <c r="D28" t="n">
-        <v>0.002</v>
+        <v>0.427</v>
       </c>
       <c r="E28" t="n">
-        <v>0.007</v>
+        <v>0.429</v>
       </c>
       <c r="F28" t="n">
-        <v>0.007</v>
+        <v>0.54</v>
       </c>
       <c r="G28" t="n">
-        <v>0.011</v>
+        <v>0.681</v>
       </c>
       <c r="H28" t="n">
-        <v>0.01</v>
+        <v>0.707</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>f1_macro_std</t>
+          <t>recall_macro_mean</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1292,28 +1292,28 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.005</v>
+        <v>0.428</v>
       </c>
       <c r="D29" t="n">
-        <v>0.004</v>
+        <v>0.402</v>
       </c>
       <c r="E29" t="n">
-        <v>0.005</v>
+        <v>0.447</v>
       </c>
       <c r="F29" t="n">
-        <v>0.007</v>
+        <v>0.572</v>
       </c>
       <c r="G29" t="n">
-        <v>0.004</v>
+        <v>0.6909999999999999</v>
       </c>
       <c r="H29" t="n">
-        <v>0.017</v>
+        <v>0.722</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>recall_micro_mean</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1337,13 +1337,13 @@
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>recall_micro_mean</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1352,28 +1352,28 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.014</v>
+        <v>0.342</v>
       </c>
       <c r="D31" t="n">
-        <v>0.012</v>
+        <v>0.297</v>
       </c>
       <c r="E31" t="n">
-        <v>0.016</v>
+        <v>0.337</v>
       </c>
       <c r="F31" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.36</v>
       </c>
       <c r="G31" t="n">
-        <v>0.02</v>
+        <v>0.43</v>
       </c>
       <c r="H31" t="n">
-        <v>0.016</v>
+        <v>0.542</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>recall_micro_mean</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1382,28 +1382,28 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.012</v>
+        <v>0.454</v>
       </c>
       <c r="D32" t="n">
-        <v>0.014</v>
+        <v>0.434</v>
       </c>
       <c r="E32" t="n">
-        <v>0.004</v>
+        <v>0.406</v>
       </c>
       <c r="F32" t="n">
-        <v>0.012</v>
+        <v>0.508</v>
       </c>
       <c r="G32" t="n">
-        <v>0.01</v>
+        <v>0.594</v>
       </c>
       <c r="H32" t="n">
-        <v>0.015</v>
+        <v>0.569</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>recall_micro_mean</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1412,28 +1412,28 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.007</v>
+        <v>0.469</v>
       </c>
       <c r="D33" t="n">
-        <v>0.004</v>
+        <v>0.49</v>
       </c>
       <c r="E33" t="n">
-        <v>0.004</v>
+        <v>0.47</v>
       </c>
       <c r="F33" t="n">
-        <v>0.003</v>
+        <v>0.537</v>
       </c>
       <c r="G33" t="n">
-        <v>0.015</v>
+        <v>0.602</v>
       </c>
       <c r="H33" t="n">
-        <v>0.021</v>
+        <v>0.594</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>recall_micro_mean</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1442,28 +1442,28 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.004</v>
+        <v>0.475</v>
       </c>
       <c r="D34" t="n">
-        <v>0.006</v>
+        <v>0.513</v>
       </c>
       <c r="E34" t="n">
-        <v>0.005</v>
+        <v>0.511</v>
       </c>
       <c r="F34" t="n">
-        <v>0.004</v>
+        <v>0.584</v>
       </c>
       <c r="G34" t="n">
-        <v>0.004</v>
+        <v>0.665</v>
       </c>
       <c r="H34" t="n">
-        <v>0.008</v>
+        <v>0.639</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>recall_micro_mean</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1472,28 +1472,28 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.004</v>
+        <v>0.473</v>
       </c>
       <c r="D35" t="n">
-        <v>0.005</v>
+        <v>0.513</v>
       </c>
       <c r="E35" t="n">
-        <v>0.005</v>
+        <v>0.536</v>
       </c>
       <c r="F35" t="n">
-        <v>0.001</v>
+        <v>0.59</v>
       </c>
       <c r="G35" t="n">
-        <v>0.008</v>
+        <v>0.696</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01</v>
+        <v>0.669</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>f1_micro_std</t>
+          <t>recall_micro_mean</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1502,28 +1502,28 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.002</v>
+        <v>0.5659999999999999</v>
       </c>
       <c r="D36" t="n">
-        <v>0.002</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="E36" t="n">
-        <v>0.003</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F36" t="n">
-        <v>0.004</v>
+        <v>0.612</v>
       </c>
       <c r="G36" t="n">
-        <v>0.001</v>
+        <v>0.7</v>
       </c>
       <c r="H36" t="n">
-        <v>0.007</v>
+        <v>0.699</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>accuracy_balanced_std</t>
+          <t>precision_macro_mean</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1547,13 +1547,13 @@
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>0.402</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>accuracy_balanced_std</t>
+          <t>precision_macro_mean</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1562,28 +1562,28 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.001</v>
+        <v>0.276</v>
       </c>
       <c r="D38" t="n">
-        <v>0.007</v>
+        <v>0.178</v>
       </c>
       <c r="E38" t="n">
-        <v>0.007</v>
+        <v>0.187</v>
       </c>
       <c r="F38" t="n">
-        <v>0.006</v>
+        <v>0.271</v>
       </c>
       <c r="G38" t="n">
-        <v>0.023</v>
+        <v>0.214</v>
       </c>
       <c r="H38" t="n">
-        <v>0.014</v>
+        <v>0.499</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>accuracy_balanced_std</t>
+          <t>precision_macro_mean</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1592,28 +1592,28 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.02</v>
+        <v>0.383</v>
       </c>
       <c r="D39" t="n">
-        <v>0.014</v>
+        <v>0.437</v>
       </c>
       <c r="E39" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.346</v>
       </c>
       <c r="F39" t="n">
-        <v>0.017</v>
+        <v>0.437</v>
       </c>
       <c r="G39" t="n">
-        <v>0.02</v>
+        <v>0.51</v>
       </c>
       <c r="H39" t="n">
-        <v>0.014</v>
+        <v>0.507</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>accuracy_balanced_std</t>
+          <t>precision_macro_mean</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1622,28 +1622,28 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.399</v>
       </c>
       <c r="D40" t="n">
-        <v>0.004</v>
+        <v>0.439</v>
       </c>
       <c r="E40" t="n">
-        <v>0.01</v>
+        <v>0.431</v>
       </c>
       <c r="F40" t="n">
-        <v>0.016</v>
+        <v>0.484</v>
       </c>
       <c r="G40" t="n">
-        <v>0.018</v>
+        <v>0.544</v>
       </c>
       <c r="H40" t="n">
-        <v>0.004</v>
+        <v>0.527</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>accuracy_balanced_std</t>
+          <t>precision_macro_mean</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1652,28 +1652,28 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.001</v>
+        <v>0.391</v>
       </c>
       <c r="D41" t="n">
-        <v>0.001</v>
+        <v>0.425</v>
       </c>
       <c r="E41" t="n">
-        <v>0.01</v>
+        <v>0.485</v>
       </c>
       <c r="F41" t="n">
-        <v>0.007</v>
+        <v>0.58</v>
       </c>
       <c r="G41" t="n">
-        <v>0.024</v>
+        <v>0.665</v>
       </c>
       <c r="H41" t="n">
-        <v>0.014</v>
+        <v>0.569</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>accuracy_balanced_std</t>
+          <t>precision_macro_mean</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1682,52 +1682,2572 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.003</v>
+        <v>0.389</v>
       </c>
       <c r="D42" t="n">
-        <v>0.004</v>
+        <v>0.414</v>
       </c>
       <c r="E42" t="n">
-        <v>0.008</v>
+        <v>0.516</v>
       </c>
       <c r="F42" t="n">
-        <v>0.005</v>
+        <v>0.572</v>
       </c>
       <c r="G42" t="n">
-        <v>0.006</v>
+        <v>0.697</v>
       </c>
       <c r="H42" t="n">
-        <v>0.003</v>
+        <v>0.593</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
+          <t>precision_macro_mean</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.509</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.617</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.696</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0.632</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_mean</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0.425</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_mean</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>0.342</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.337</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0.542</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_mean</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>0.454</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.434</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.406</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.508</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.594</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.569</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_mean</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0.469</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.537</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.602</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.594</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_mean</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.511</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.584</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.665</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.639</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_mean</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>0.473</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.536</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.696</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.669</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_mean</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0.5659999999999999</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.5629999999999999</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.612</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.699</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_mean</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_mean</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>0.242</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.186</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.273</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.359</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_mean</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.356</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.444</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.534</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_mean</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>0.405</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.427</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.405</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_mean</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>0.416</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.534</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.629</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.605</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_mean</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0.415</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.479</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.662</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.638</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_mean</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.667</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.669</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_mean</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.389</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_mean</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>0.249</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.193</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.253</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.363</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.504</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_mean</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.551</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_mean</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>0.406</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.428</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.406</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.481</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.5610000000000001</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.5649999999999999</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_mean</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>0.417</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.535</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.607</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_mean</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0.415</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.464</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.545</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.663</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_mean</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0.514</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>f1_macro_std</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>0</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>f1_macro_std</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>0</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>f1_macro_std</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>f1_macro_std</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>f1_macro_std</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>f1_macro_std</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>f1_macro_std</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.017</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>accuracy/f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>accuracy/f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>accuracy/f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>accuracy/f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>accuracy/f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>accuracy/f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>accuracy/f1_micro_std</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.007</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
           <t>accuracy_balanced_std</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>0</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D80" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D81" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="D82" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F82" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="H82" t="n">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D83" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F83" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G83" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="H83" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D84" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F84" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G84" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="H84" t="n">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>accuracy_balanced_std</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
         <is>
           <t>10000</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="C85" t="n">
         <v>0.004</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D85" t="n">
         <v>0.003</v>
       </c>
-      <c r="E43" t="n">
+      <c r="E85" t="n">
         <v>0.005</v>
       </c>
-      <c r="F43" t="n">
+      <c r="F85" t="n">
         <v>0.008999999999999999</v>
       </c>
-      <c r="G43" t="n">
+      <c r="G85" t="n">
         <v>0.02</v>
       </c>
-      <c r="H43" t="n">
+      <c r="H85" t="n">
         <v>0.013</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>recall_macro_std</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>recall_macro_std</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D87" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="F87" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="G87" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>recall_macro_std</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D88" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="E88" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="F88" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="G88" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H88" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>recall_macro_std</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="D89" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F89" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="G89" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="H89" t="n">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>recall_macro_std</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D90" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="F90" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>recall_macro_std</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D91" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E91" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="F91" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G91" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="H91" t="n">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>recall_macro_std</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D92" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="E92" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F92" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G92" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H92" t="n">
+        <v>0.013</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>recall_micro_std</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>0</v>
+      </c>
+      <c r="D93" t="n">
+        <v>0</v>
+      </c>
+      <c r="E93" t="n">
+        <v>0</v>
+      </c>
+      <c r="F93" t="n">
+        <v>0</v>
+      </c>
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>recall_micro_std</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="D94" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E94" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="F94" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G94" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>recall_micro_std</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="D95" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="E95" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F95" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="G95" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>recall_micro_std</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="D96" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E96" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F96" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="G96" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H96" t="n">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>recall_micro_std</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D97" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E97" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F97" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G97" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>recall_micro_std</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D98" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E98" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F98" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G98" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H98" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>recall_micro_std</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D99" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E99" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F99" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G99" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H99" t="n">
+        <v>0.007</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>precision_macro_std</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>0</v>
+      </c>
+      <c r="D100" t="n">
+        <v>0</v>
+      </c>
+      <c r="E100" t="n">
+        <v>0</v>
+      </c>
+      <c r="F100" t="n">
+        <v>0</v>
+      </c>
+      <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>precision_macro_std</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="D101" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="E101" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="F101" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H101" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>precision_macro_std</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="F102" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>precision_macro_std</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="D103" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="E103" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="F103" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="H103" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>precision_macro_std</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="D104" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="E104" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="F104" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="H104" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>precision_macro_std</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D105" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F105" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="H105" t="n">
+        <v>0.006</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>precision_macro_std</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D106" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="E106" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F106" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G106" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="H106" t="n">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_std</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>0</v>
+      </c>
+      <c r="D107" t="n">
+        <v>0</v>
+      </c>
+      <c r="E107" t="n">
+        <v>0</v>
+      </c>
+      <c r="F107" t="n">
+        <v>0</v>
+      </c>
+      <c r="G107" t="n">
+        <v>0</v>
+      </c>
+      <c r="H107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_std</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="D108" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="E108" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="F108" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G108" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H108" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_std</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="D109" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="E109" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F109" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="G109" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H109" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_std</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="D110" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E110" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="F110" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="H110" t="n">
+        <v>0.021</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_std</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D111" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E111" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F111" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G111" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H111" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_std</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D112" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="E112" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F112" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H112" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>precision_micro_std</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D113" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E113" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F113" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H113" t="n">
+        <v>0.007</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_std</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>0</v>
+      </c>
+      <c r="D114" t="n">
+        <v>0</v>
+      </c>
+      <c r="E114" t="n">
+        <v>0</v>
+      </c>
+      <c r="F114" t="n">
+        <v>0</v>
+      </c>
+      <c r="G114" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_std</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="D115" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="E115" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="F115" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G115" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="H115" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_std</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="D116" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E116" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F116" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="H116" t="n">
+        <v>0.016</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_std</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="D117" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E117" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F117" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="H117" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_std</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D118" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="E118" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F118" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H118" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_std</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D119" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E119" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F119" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H119" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="inlineStr">
+        <is>
+          <t>cohen_kappa_std</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D120" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E120" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F120" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H120" t="n">
+        <v>0.007</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_std</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>0</v>
+      </c>
+      <c r="D121" t="n">
+        <v>0</v>
+      </c>
+      <c r="E121" t="n">
+        <v>0</v>
+      </c>
+      <c r="F121" t="n">
+        <v>0</v>
+      </c>
+      <c r="G121" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_std</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="D122" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="E122" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="F122" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G122" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="H122" t="n">
+        <v>0.015</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_std</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="D123" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E123" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F123" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G123" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="H123" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_std</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="D124" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E124" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F124" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G124" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="H124" t="n">
+        <v>0.018</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_std</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="D125" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="E125" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F125" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G125" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="H125" t="n">
+        <v>0.008</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_std</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="D126" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="E126" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="F126" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="G126" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H126" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="inlineStr">
+        <is>
+          <t>matthews_corrcoef_std</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="D127" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E127" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="F127" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="G127" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H127" t="n">
+        <v>0.007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug where for cap-sotu one data interval was 3000 instead of 5000 specifically for logistic (not other algos). new data uploaded
</commit_message>
<xml_diff>
--- a/appendix/metrics_all_cap-sotu.xlsx
+++ b/appendix/metrics_all_cap-sotu.xlsx
@@ -628,7 +628,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -838,11 +838,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.485</v>
+        <v>0.501</v>
       </c>
       <c r="D14" t="n">
         <v>0.54</v>
@@ -1048,11 +1048,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.349</v>
+        <v>0.344</v>
       </c>
       <c r="D21" t="n">
         <v>0.378</v>
@@ -1258,11 +1258,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.473</v>
+        <v>0.476</v>
       </c>
       <c r="D28" t="n">
         <v>0.513</v>
@@ -1468,11 +1468,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.378</v>
+        <v>0.388</v>
       </c>
       <c r="D35" t="n">
         <v>0.427</v>
@@ -1678,11 +1678,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.378</v>
+        <v>0.388</v>
       </c>
       <c r="D42" t="n">
         <v>0.427</v>
@@ -1888,11 +1888,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.473</v>
+        <v>0.476</v>
       </c>
       <c r="D49" t="n">
         <v>0.513</v>
@@ -2098,11 +2098,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.477</v>
+        <v>0.484</v>
       </c>
       <c r="D56" t="n">
         <v>0.518</v>
@@ -2308,11 +2308,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0.349</v>
+        <v>0.36</v>
       </c>
       <c r="D63" t="n">
         <v>0.401</v>
@@ -2518,11 +2518,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.389</v>
+        <v>0.377</v>
       </c>
       <c r="D70" t="n">
         <v>0.414</v>
@@ -2728,11 +2728,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.473</v>
+        <v>0.476</v>
       </c>
       <c r="D77" t="n">
         <v>0.513</v>
@@ -2938,11 +2938,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.501</v>
+        <v>0.52</v>
       </c>
       <c r="D84" t="n">
         <v>0.5669999999999999</v>
@@ -3148,11 +3148,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0.357</v>
+        <v>0.335</v>
       </c>
       <c r="D91" t="n">
         <v>0.368</v>
@@ -3358,11 +3358,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.498</v>
+        <v>0.497</v>
       </c>
       <c r="D98" t="n">
         <v>0.526</v>
@@ -3568,11 +3568,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0.432</v>
+        <v>0.442</v>
       </c>
       <c r="D105" t="n">
         <v>0.492</v>
@@ -3778,11 +3778,11 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>0.415</v>
+        <v>0.421</v>
       </c>
       <c r="D112" t="n">
         <v>0.463</v>
@@ -3988,11 +3988,11 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>0.415</v>
+        <v>0.422</v>
       </c>
       <c r="D119" t="n">
         <v>0.464</v>
@@ -4198,11 +4198,11 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="D126" t="n">
         <v>0.002</v>
@@ -4408,11 +4408,11 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="D133" t="n">
         <v>0.01</v>
@@ -4618,7 +4618,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -4828,11 +4828,11 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="D147" t="n">
         <v>0.005</v>
@@ -5038,11 +5038,11 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="D154" t="n">
         <v>0.004</v>
@@ -5248,11 +5248,11 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="D161" t="n">
         <v>0.004</v>
@@ -5458,11 +5458,11 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C168" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="D168" t="n">
         <v>0.005</v>
@@ -5668,11 +5668,11 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C175" t="n">
-        <v>0.006</v>
+        <v>0.003</v>
       </c>
       <c r="D175" t="n">
         <v>0.008999999999999999</v>
@@ -5878,11 +5878,11 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C182" t="n">
-        <v>0.004</v>
+        <v>0.006</v>
       </c>
       <c r="D182" t="n">
         <v>0.003</v>
@@ -6088,11 +6088,11 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0.005</v>
+        <v>0.003</v>
       </c>
       <c r="D189" t="n">
         <v>0.007</v>
@@ -6298,11 +6298,11 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C196" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="D196" t="n">
         <v>0.005</v>
@@ -6508,11 +6508,11 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C203" t="n">
-        <v>0.007</v>
+        <v>0.003</v>
       </c>
       <c r="D203" t="n">
         <v>0.012</v>
@@ -6718,11 +6718,11 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>0.008</v>
+        <v>0.004</v>
       </c>
       <c r="D210" t="n">
         <v>0.012</v>
@@ -6928,11 +6928,11 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>0.007</v>
+        <v>0.002</v>
       </c>
       <c r="D217" t="n">
         <v>0.008999999999999999</v>
@@ -7138,11 +7138,11 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C224" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="D224" t="n">
         <v>0.002</v>
@@ -7348,7 +7348,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C231" t="n">
@@ -7558,7 +7558,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="C238" t="n">

</xml_diff>